<commit_message>
Added Timesheet of date 29-01-2020
</commit_message>
<xml_diff>
--- a/Timesheet January 2020.xlsx
+++ b/Timesheet January 2020.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\Timesheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F252B11-B543-4C5A-89A3-45269E200BBA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83077FFB-44A5-4B90-992A-16477159326C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{4E06B61D-CC95-4C6D-96A7-14002220E881}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="39">
   <si>
     <t>Timestamp</t>
   </si>
@@ -95,6 +95,70 @@
   </si>
   <si>
     <t>Jan 28 18:00 to 19:00</t>
+  </si>
+  <si>
+    <t>Jan 29 10:00 to 11:00</t>
+  </si>
+  <si>
+    <t>Jan 29 11:00 to 12:00</t>
+  </si>
+  <si>
+    <t>Modified code of saving output graphs, now graphs are not saved.
+Applied two pair z-test</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Applied 1 paired z-test on good day and data file values. </t>
+  </si>
+  <si>
+    <t>Jan 29 12:00 to 13:00</t>
+  </si>
+  <si>
+    <t>Applied f-test. Applying anova test, modifieying data according to
+anova table. Performed missing values imputation.</t>
+  </si>
+  <si>
+    <t>Performed Anova test, printed anova table. Applied anova test of
+assumptions by using Levene test and Shapiro-Wilk test.</t>
+  </si>
+  <si>
+    <t>Jan 29 13:00 to 13:30</t>
+  </si>
+  <si>
+    <t>Jan 29 13:30 to 14:00</t>
+  </si>
+  <si>
+    <t>Observation and result documentation of statistical tests.</t>
+  </si>
+  <si>
+    <t>Jan 29 14:00 to 15:00</t>
+  </si>
+  <si>
+    <t>Python Class</t>
+  </si>
+  <si>
+    <t>Jan 29 15:00 to 16:00</t>
+  </si>
+  <si>
+    <t>Searching slution for doing timeseries analysis</t>
+  </si>
+  <si>
+    <t>Jan 29 16:00 to 17:00</t>
+  </si>
+  <si>
+    <t>Visualization of both machine timeseries</t>
+  </si>
+  <si>
+    <t>Jan 29 17:00 to 18:00</t>
+  </si>
+  <si>
+    <t>Timeseries decomposition, modeified code of timeseries saving.</t>
+  </si>
+  <si>
+    <t>Jan 29 18:00 to 19:00</t>
+  </si>
+  <si>
+    <t>Found errors when decomposing timeseries data. Tryed converting
+data by interpolation and converting date to datetime.</t>
   </si>
 </sst>
 </file>
@@ -119,7 +183,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.39997558519241921"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -144,17 +208,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -470,27 +534,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07624C4B-536F-4CB7-AB8E-70C51D83A0BA}">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="25.85546875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="61.5703125" style="5" customWidth="1"/>
+    <col min="2" max="2" width="61.5703125" style="3" customWidth="1"/>
     <col min="3" max="3" width="22.5703125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="5" t="s">
         <v>3</v>
       </c>
     </row>
@@ -509,7 +573,7 @@
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C3" s="1" t="s">
@@ -528,7 +592,7 @@
       </c>
     </row>
     <row r="5" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="4" t="s">
         <v>11</v>
       </c>
       <c r="B5" s="2" t="s">
@@ -561,13 +625,128 @@
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="3" t="s">
         <v>17</v>
       </c>
       <c r="C8" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="5"/>
+      <c r="B9" s="6"/>
+      <c r="C9" s="5"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C19" s="1" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added MOM of date Jan 30 2020
</commit_message>
<xml_diff>
--- a/Timesheet January 2020.xlsx
+++ b/Timesheet January 2020.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\Timesheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83077FFB-44A5-4B90-992A-16477159326C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{766CDB88-C637-47C6-A9A7-BB7AB407B18B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{4E06B61D-CC95-4C6D-96A7-14002220E881}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="55">
   <si>
     <t>Timestamp</t>
   </si>
@@ -159,6 +159,59 @@
   <si>
     <t>Found errors when decomposing timeseries data. Tryed converting
 data by interpolation and converting date to datetime.</t>
+  </si>
+  <si>
+    <t>Jan 30 10:00 to 12:00</t>
+  </si>
+  <si>
+    <t>Client call</t>
+  </si>
+  <si>
+    <t>Sapphire automation</t>
+  </si>
+  <si>
+    <t>Jan 30 12:00 to 13:00</t>
+  </si>
+  <si>
+    <t>Discussion with nitin sir and sujata man, creating new jupyter 
+notebook, modifying code of good days buckets to be saved in
+specified directory.</t>
+  </si>
+  <si>
+    <t>Jan 30 13:00 to 14:00</t>
+  </si>
+  <si>
+    <t>Jan 30 14:00 to 15:00</t>
+  </si>
+  <si>
+    <t>In combined dataset notebook, cleaned good days data of both the 
+machines. Combined both datasets by performing full outer join on it.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Revising percentile concent by watching call recording. Creating
+percentile buckets. </t>
+  </si>
+  <si>
+    <t>Jan 30 15:00 to 16:00</t>
+  </si>
+  <si>
+    <t>Jan 30 16:00 to 17:00</t>
+  </si>
+  <si>
+    <t>Python class, working on connecting output counts to combind data.</t>
+  </si>
+  <si>
+    <t>Jan 30 17:00 to 18:00</t>
+  </si>
+  <si>
+    <t>Combined output data with previously combined dataset.</t>
+  </si>
+  <si>
+    <t>Jan 30 18:00 to 19:00</t>
+  </si>
+  <si>
+    <t>Python class, Connected output counts to combined data, working on
+percentile concepts by picking up examples.</t>
   </si>
 </sst>
 </file>
@@ -174,7 +227,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -184,6 +237,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -200,7 +259,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -218,6 +277,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -534,16 +599,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07624C4B-536F-4CB7-AB8E-70C51D83A0BA}">
-  <dimension ref="A1:C19"/>
+  <dimension ref="A1:C28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="25.85546875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="61.5703125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="62.85546875" style="3" customWidth="1"/>
     <col min="3" max="3" width="22.5703125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -636,9 +701,9 @@
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="5"/>
-      <c r="B9" s="6"/>
-      <c r="C9" s="5"/>
+      <c r="A9" s="7"/>
+      <c r="B9" s="8"/>
+      <c r="C9" s="7"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
@@ -747,6 +812,99 @@
         <v>38</v>
       </c>
       <c r="C19" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="5"/>
+      <c r="B20" s="6"/>
+      <c r="C20" s="5"/>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A28" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C28" s="1" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added timesheet of date 31-01-2020
</commit_message>
<xml_diff>
--- a/Timesheet January 2020.xlsx
+++ b/Timesheet January 2020.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\Timesheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{766CDB88-C637-47C6-A9A7-BB7AB407B18B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07B1B914-A333-4840-B519-737A55D55608}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{4E06B61D-CC95-4C6D-96A7-14002220E881}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="64">
   <si>
     <t>Timestamp</t>
   </si>
@@ -212,6 +212,39 @@
   <si>
     <t>Python class, Connected output counts to combined data, working on
 percentile concepts by picking up examples.</t>
+  </si>
+  <si>
+    <t>Jan 31 10:00 to 11:00</t>
+  </si>
+  <si>
+    <t>Trying to convert buckets to dictionaries but the format of buckets
+sample is conflicted while writing to dict. No json or ast methods are
+applicable to it. Working on another solution to re-create it.</t>
+  </si>
+  <si>
+    <t>Jan 31 11:00 to 12:00</t>
+  </si>
+  <si>
+    <t>Figured out solution of loading buckets as dictionaries by transforming
+buckets to list from data exploration of sysytem health file. Using json
+loads to make bucket into dictionary. For this modified code creation 
+of bucket data by writing starting and ending time as string.</t>
+  </si>
+  <si>
+    <t>Jan 31 12:00 to 13:00</t>
+  </si>
+  <si>
+    <t>Creating percentile buckets</t>
+  </si>
+  <si>
+    <t>Jan 31 13:00 to 14:00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Created percentile buckets, choosed percentile as 80, facing some 
+issues regarding of nan values. </t>
+  </si>
+  <si>
+    <t>Jan 31 14:00 to 15:00</t>
   </si>
 </sst>
 </file>
@@ -599,10 +632,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07624C4B-536F-4CB7-AB8E-70C51D83A0BA}">
-  <dimension ref="A1:C28"/>
+  <dimension ref="A1:C34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -908,6 +941,66 @@
         <v>8</v>
       </c>
     </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="5"/>
+      <c r="B29" s="6"/>
+      <c r="C29" s="5"/>
+    </row>
+    <row r="30" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="105" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added MOM of date 31-01-2020
</commit_message>
<xml_diff>
--- a/Timesheet January 2020.xlsx
+++ b/Timesheet January 2020.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\Timesheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07B1B914-A333-4840-B519-737A55D55608}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04D743A2-0CBF-4FA0-A744-BFDBD909AF8B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{4E06B61D-CC95-4C6D-96A7-14002220E881}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="72">
   <si>
     <t>Timestamp</t>
   </si>
@@ -245,6 +245,30 @@
   </si>
   <si>
     <t>Jan 31 14:00 to 15:00</t>
+  </si>
+  <si>
+    <t>Jan 31 15:00 to 16:00</t>
+  </si>
+  <si>
+    <t>Build sample multiple linear regression model.</t>
+  </si>
+  <si>
+    <t>Jan 31 16:00 to 17:00</t>
+  </si>
+  <si>
+    <t>Build linear regression model using sklearn.linear regresion</t>
+  </si>
+  <si>
+    <t>Jan 31 17:00 to 18:00</t>
+  </si>
+  <si>
+    <t>Seached about other predictive model. Undertanding features of data.</t>
+  </si>
+  <si>
+    <t>Jan 31 18:00 to 19:00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Applied MLP neural network. Results were all same values. Need to fix this problem because further neural network strategy will be used for prediction. </t>
   </si>
 </sst>
 </file>
@@ -632,10 +656,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07624C4B-536F-4CB7-AB8E-70C51D83A0BA}">
-  <dimension ref="A1:C34"/>
+  <dimension ref="A1:C38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="D38" sqref="D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -837,7 +861,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>37</v>
       </c>
@@ -1001,6 +1025,50 @@
         <v>8</v>
       </c>
     </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added timesheet of date 06-02-2020
</commit_message>
<xml_diff>
--- a/Timesheet January 2020.xlsx
+++ b/Timesheet January 2020.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\Timesheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04D743A2-0CBF-4FA0-A744-BFDBD909AF8B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45355A99-AA20-464F-83CB-5804E37A0763}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{4E06B61D-CC95-4C6D-96A7-14002220E881}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="147">
   <si>
     <t>Timestamp</t>
   </si>
@@ -269,6 +269,253 @@
   </si>
   <si>
     <t xml:space="preserve">Applied MLP neural network. Results were all same values. Need to fix this problem because further neural network strategy will be used for prediction. </t>
+  </si>
+  <si>
+    <t>Feb 03 10:00 to 11:00</t>
+  </si>
+  <si>
+    <t>Created features: max event occur, max sublocation occur, min
+sublocation occur, alarm duration.</t>
+  </si>
+  <si>
+    <t>Feb 03 11:00 to 12:00</t>
+  </si>
+  <si>
+    <t>Created features: day of week, day of month and month of year.</t>
+  </si>
+  <si>
+    <t>Feb 03 12:00 to 13:00</t>
+  </si>
+  <si>
+    <t>Filled na values of max event occur with event close to mean of 
+events.</t>
+  </si>
+  <si>
+    <t>Feb 03 13:00 to 14:00</t>
+  </si>
+  <si>
+    <t>Structurized problem statement. Understood input variables, output
+variables and at what factors output should be evaluated. Understood
+categorical attributes in dataset. Converting the categorical values to
+numerical using label encoding method.</t>
+  </si>
+  <si>
+    <t>Feb 03 14:00 to 15:00</t>
+  </si>
+  <si>
+    <t>Feb 03 14:00 to 14:30</t>
+  </si>
+  <si>
+    <t>Applied label encoding to categorical columns.</t>
+  </si>
+  <si>
+    <t>Feb 03 15:00 to 16:00</t>
+  </si>
+  <si>
+    <t>Applied multi output regression model. Generated train-test split.
+Used train-test ratio as 70:30</t>
+  </si>
+  <si>
+    <t>Feb 03 16:00 to 17:00</t>
+  </si>
+  <si>
+    <t>Applied SVM algo. Checked model accuracy after it.</t>
+  </si>
+  <si>
+    <t>Feb 03 17:00 to 18:00</t>
+  </si>
+  <si>
+    <t>Printed model accuracy of both the algorithms.</t>
+  </si>
+  <si>
+    <t>Feb 03 18:00 to 19:00</t>
+  </si>
+  <si>
+    <t>Working on scalling because of results of predictions were not good.
+Geeting join conflicts while concatinating scaled and non scaled data.
+Working on finding best hyperparametrs and also applying deep
+learning techniques.</t>
+  </si>
+  <si>
+    <t>Feb 04 10:00 to 11:00</t>
+  </si>
+  <si>
+    <t>Feb 04 11:00 to 12:00</t>
+  </si>
+  <si>
+    <t>Aplied KNN regressor on dataset for prediction. Visualized RMSE from
+k equals 1 to 50.</t>
+  </si>
+  <si>
+    <t>Scaled input variable within various ranges every time. The results
+were not great. Using KNN regresor for prediction.</t>
+  </si>
+  <si>
+    <t>Found best hyperparameters for knn. Finding best hyperparameters
+for random forest.</t>
+  </si>
+  <si>
+    <t>Feb 04 12:00 to 13:00</t>
+  </si>
+  <si>
+    <t>Feb 04 13:30 to 14:00</t>
+  </si>
+  <si>
+    <t>Printed best hyperparameters of knn and random forest.</t>
+  </si>
+  <si>
+    <t>Feb 04 14:00 to 15:00</t>
+  </si>
+  <si>
+    <t>Generating sample predictions</t>
+  </si>
+  <si>
+    <t>Feb 04 15:00 to 16:00</t>
+  </si>
+  <si>
+    <t>Choosed random forest regressor for building model. Generated
+sample prediction on data.</t>
+  </si>
+  <si>
+    <t>Feb 04 16:00 to 17:00</t>
+  </si>
+  <si>
+    <t>Undertanding tensorflow for modeling regresion problem. Solving an
+example to understand prediction using tensorflow and keras.</t>
+  </si>
+  <si>
+    <t>Feb 04 17:00 to 18:00</t>
+  </si>
+  <si>
+    <t>Understanding tensorflow for regression problems.</t>
+  </si>
+  <si>
+    <t>Feb 04 18:00 to 19:00</t>
+  </si>
+  <si>
+    <t>Understand and applied neural to dataset.</t>
+  </si>
+  <si>
+    <t>Feb 05 10:00 to 11:00</t>
+  </si>
+  <si>
+    <t>Modified some code of combined analysis. Added doc strings in
+functions.</t>
+  </si>
+  <si>
+    <t>Feb 05 11:00 to 12:00</t>
+  </si>
+  <si>
+    <t>Modifying logic of imputing null values. Writen function which
+imputes null value with random value picked within range mean - std
+and mean + std.</t>
+  </si>
+  <si>
+    <t>Feb 05 12:00 to 13:00</t>
+  </si>
+  <si>
+    <t>Tried every possible way to impute value using above function, but
+every time got error.</t>
+  </si>
+  <si>
+    <t>Feb 05 13:00 to 13:30</t>
+  </si>
+  <si>
+    <t>Done imputing na values using above function.</t>
+  </si>
+  <si>
+    <t>Feb 05 13:30 to 14:00</t>
+  </si>
+  <si>
+    <t>Feb 05 14:00 to 15:00</t>
+  </si>
+  <si>
+    <t>Corrected code for filling na using above funcion. Modefied code of
+filling na of categorical columns.</t>
+  </si>
+  <si>
+    <t>Feb 05 15:00 to 16:00</t>
+  </si>
+  <si>
+    <t>Understanding regresion for deep learning.</t>
+  </si>
+  <si>
+    <t>Feb 05 16:00 to 17:00</t>
+  </si>
+  <si>
+    <t>Installed tensorflow and doing tensorflow regression example</t>
+  </si>
+  <si>
+    <t>Feb 05 17:00 to 18:00</t>
+  </si>
+  <si>
+    <t>Feb 05 18:00 to 19:00</t>
+  </si>
+  <si>
+    <t>Tensorflow caused problem while importing or loading</t>
+  </si>
+  <si>
+    <t>Solved sample examples of temsorflow, caused error while programming. Class</t>
+  </si>
+  <si>
+    <t>Feb 06 10:00 to 11:00</t>
+  </si>
+  <si>
+    <t>Checking colinerity and covariance of variables.</t>
+  </si>
+  <si>
+    <t>Feb 06 11:00 to 12:00</t>
+  </si>
+  <si>
+    <t>Plotter scater plot of some variables and checked colinearity. Found the reason why
+total output count results were poor because of no proper relationship with other
+variables.</t>
+  </si>
+  <si>
+    <t>Feb 06 12:00 to 13:00</t>
+  </si>
+  <si>
+    <t>Documented observations and solutions.</t>
+  </si>
+  <si>
+    <t>Feb 06 13:00 to 13:30</t>
+  </si>
+  <si>
+    <t>Practicing simple neural network</t>
+  </si>
+  <si>
+    <t>Feb 06 13:30 to 14:00</t>
+  </si>
+  <si>
+    <t>Feb 06 14:00 to 15:00</t>
+  </si>
+  <si>
+    <t>Practicing neural network, implemented neural network class with fit, activation and
+training functionalities.</t>
+  </si>
+  <si>
+    <t>Feb 06 15:00 to 16:00</t>
+  </si>
+  <si>
+    <t>Implemented simple neural network program. Added functionality for tanh activation.</t>
+  </si>
+  <si>
+    <t>Feb 06 16:00 to 17:00</t>
+  </si>
+  <si>
+    <t>Implemented rmse and mse accuracy functionality.</t>
+  </si>
+  <si>
+    <t>Feb 06 17:00 to 18:00</t>
+  </si>
+  <si>
+    <t>Implemented multi layer perceptron. Added functionalities of dot product and activation</t>
+  </si>
+  <si>
+    <t>Feb 06 18:00 to 19:00</t>
+  </si>
+  <si>
+    <t>Implemented back propagation for MLP.</t>
   </si>
 </sst>
 </file>
@@ -316,7 +563,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -341,6 +588,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -656,16 +906,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07624C4B-536F-4CB7-AB8E-70C51D83A0BA}">
-  <dimension ref="A1:C38"/>
+  <dimension ref="A1:C81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="D38" sqref="D38"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="B77" sqref="B77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="25.85546875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="62.85546875" style="3" customWidth="1"/>
+    <col min="2" max="2" width="79.42578125" style="3" customWidth="1"/>
     <col min="3" max="3" width="22.5703125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1069,6 +1319,455 @@
         <v>8</v>
       </c>
     </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="5"/>
+      <c r="B39" s="6"/>
+      <c r="C39" s="5"/>
+    </row>
+    <row r="40" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" ht="105" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" s="5"/>
+      <c r="B50" s="6"/>
+      <c r="C50" s="5"/>
+    </row>
+    <row r="51" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A51" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A52" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A53" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="B54" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B55" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A56" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A57" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B58" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B59" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" s="5"/>
+      <c r="B60" s="6"/>
+      <c r="C60" s="5"/>
+    </row>
+    <row r="61" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A61" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A62" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A63" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B64" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B65" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A66" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B66" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B67" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B68" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B69" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A70" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="B70" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A71" s="5"/>
+      <c r="B71" s="6"/>
+      <c r="C71" s="5"/>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A72" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="B72" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A73" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="B73" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A74" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="B74" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A75" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="B75" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A76" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="B76" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C76" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A77" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="B77" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="C77" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A78" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="B78" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="C78" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A79" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="B79" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="C79" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A80" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="B80" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="C80" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A81" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="B81" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="C81" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added timesheet information of date 07-02-2020
</commit_message>
<xml_diff>
--- a/Timesheet January 2020.xlsx
+++ b/Timesheet January 2020.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\Timesheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45355A99-AA20-464F-83CB-5804E37A0763}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{824BED57-65B7-4D90-A7EF-5E7C5532B6D7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{4E06B61D-CC95-4C6D-96A7-14002220E881}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="164">
   <si>
     <t>Timestamp</t>
   </si>
@@ -516,6 +516,57 @@
   </si>
   <si>
     <t>Implemented back propagation for MLP.</t>
+  </si>
+  <si>
+    <t>Feb 07 10:00 to 11:00</t>
+  </si>
+  <si>
+    <t>Sapphire Automation</t>
+  </si>
+  <si>
+    <t>Feb 07 11:00 to 12:00</t>
+  </si>
+  <si>
+    <t>Practicing neural network on local machine.</t>
+  </si>
+  <si>
+    <t>Feb 07 12:00 to 13:00</t>
+  </si>
+  <si>
+    <t>Used OOP concepts of inheritence and polymorphism in MLP code.</t>
+  </si>
+  <si>
+    <t>Feb 07 13:00 to 14:00</t>
+  </si>
+  <si>
+    <t>Feb 07 14:00 to 15:00</t>
+  </si>
+  <si>
+    <t>Modified logic of dot product in MLP.</t>
+  </si>
+  <si>
+    <t>Feb 07 15:00 to 16:00</t>
+  </si>
+  <si>
+    <t>Implementing back propagation in MLP.</t>
+  </si>
+  <si>
+    <t>Feb 07 16:00 to 17:00</t>
+  </si>
+  <si>
+    <t>Succesfully implemented MLP</t>
+  </si>
+  <si>
+    <t>Feb 07 17:00 to 18:00</t>
+  </si>
+  <si>
+    <t>Verified model accuracy</t>
+  </si>
+  <si>
+    <t>Feb 07 18:00 to 19:00</t>
+  </si>
+  <si>
+    <t>Model accuracy is very poor, need modification for algorithm.</t>
   </si>
 </sst>
 </file>
@@ -906,10 +957,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07624C4B-536F-4CB7-AB8E-70C51D83A0BA}">
-  <dimension ref="A1:C81"/>
+  <dimension ref="A1:C91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="B77" sqref="B77"/>
+    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
+      <selection activeCell="D91" sqref="D91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1669,7 +1720,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="73" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
         <v>130</v>
       </c>
@@ -1713,7 +1764,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="77" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
         <v>137</v>
       </c>
@@ -1765,6 +1816,110 @@
         <v>146</v>
       </c>
       <c r="C81" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A82" s="5"/>
+      <c r="B82" s="6"/>
+      <c r="C82" s="5"/>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A83" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="B83" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C83" s="1" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A84" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="B84" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="C84" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A85" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="B85" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="C85" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A86" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="B86" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C86" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A87" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B87" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="C87" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A88" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="B88" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="C88" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A89" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="B89" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="C89" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A90" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="B90" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="C90" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A91" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="B91" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="C91" s="1" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added timesheet for date 10-02-2020
</commit_message>
<xml_diff>
--- a/Timesheet January 2020.xlsx
+++ b/Timesheet January 2020.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\Timesheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{824BED57-65B7-4D90-A7EF-5E7C5532B6D7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32847B10-471D-4DA8-A0BD-10E2FAA88694}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{4E06B61D-CC95-4C6D-96A7-14002220E881}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="179">
   <si>
     <t>Timestamp</t>
   </si>
@@ -567,6 +567,52 @@
   </si>
   <si>
     <t>Model accuracy is very poor, need modification for algorithm.</t>
+  </si>
+  <si>
+    <t>Feb 10 10:00 to 11:00</t>
+  </si>
+  <si>
+    <t>Feb 10 11:00 to 12:00</t>
+  </si>
+  <si>
+    <t>Instaling project setup on my local machine but getting problems on installing
+dependencies.</t>
+  </si>
+  <si>
+    <t>Feb 10 12:00 to 13:00</t>
+  </si>
+  <si>
+    <t>Discussed with sujata mam.</t>
+  </si>
+  <si>
+    <t>Watched video that was recommeded by client.</t>
+  </si>
+  <si>
+    <t>Feb 10 13:00 to 14:00</t>
+  </si>
+  <si>
+    <t>Converted mp3 file to wav file</t>
+  </si>
+  <si>
+    <t>Feb 10 14:00 to 15:00</t>
+  </si>
+  <si>
+    <t>Program giving error while doing training and testing split. 'numpy memory error'</t>
+  </si>
+  <si>
+    <t>Feb 10 15:00 to 16:00</t>
+  </si>
+  <si>
+    <t>Feb 10 16:00 to 17:00</t>
+  </si>
+  <si>
+    <t>Looked at all the videos and understand the procedure of audio seperation.</t>
+  </si>
+  <si>
+    <t>Feb 10 17:00 to 18:00</t>
+  </si>
+  <si>
+    <t>Working on making 24 buckets rather than 1 day bin bucket.</t>
   </si>
 </sst>
 </file>
@@ -957,10 +1003,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07624C4B-536F-4CB7-AB8E-70C51D83A0BA}">
-  <dimension ref="A1:C91"/>
+  <dimension ref="A1:C100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
-      <selection activeCell="D91" sqref="D91"/>
+    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
+      <selection activeCell="C101" sqref="C101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1923,6 +1969,99 @@
         <v>8</v>
       </c>
     </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A92" s="5"/>
+      <c r="B92" s="6"/>
+      <c r="C92" s="5"/>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A93" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="B93" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="C93" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A94" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="B94" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="C94" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A95" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="B95" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="C95" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A96" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="B96" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="C96" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A97" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="B97" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C97" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A98" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="B98" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="C98" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A99" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="B99" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="C99" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A100" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="B100" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="C100" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added timesheet of date 11-02-2020
</commit_message>
<xml_diff>
--- a/Timesheet January 2020.xlsx
+++ b/Timesheet January 2020.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\Timesheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32847B10-471D-4DA8-A0BD-10E2FAA88694}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A33B0EA9-F709-43BE-9729-ABF3A3F4981E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{4E06B61D-CC95-4C6D-96A7-14002220E881}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="195">
   <si>
     <t>Timestamp</t>
   </si>
@@ -613,6 +613,54 @@
   </si>
   <si>
     <t>Working on making 24 buckets rather than 1 day bin bucket.</t>
+  </si>
+  <si>
+    <t>Feb 11 10:00 to 11:00</t>
+  </si>
+  <si>
+    <t>Uploaded timesheet of previous day to git. Working on making hourly buckets.</t>
+  </si>
+  <si>
+    <t>Feb 11 11:00 to 12:00</t>
+  </si>
+  <si>
+    <t>Using timedelta adding hour to timestamp data</t>
+  </si>
+  <si>
+    <t>Feb 11 12:00 to 13:00</t>
+  </si>
+  <si>
+    <t>Created hourly bucket, working on making the algorithm faster for hourly bucket.</t>
+  </si>
+  <si>
+    <t>Feb 11 13:00 to 14:00</t>
+  </si>
+  <si>
+    <t>Modified logic of creating hourly buckets, veryfied output by writing data in csv file.</t>
+  </si>
+  <si>
+    <t>Feb 11 14:00 to 15:00</t>
+  </si>
+  <si>
+    <t>Feb 11 15:00 to 16:00</t>
+  </si>
+  <si>
+    <t>Logic to create hourly bucket was wrong, working on new logic</t>
+  </si>
+  <si>
+    <t>Feb 11 16:00 to 17:00</t>
+  </si>
+  <si>
+    <t>Feb 11 17:00 to 18:00</t>
+  </si>
+  <si>
+    <t>Created hourly bucket, working on connecting other two files.</t>
+  </si>
+  <si>
+    <t>Feb 11 18:00 to 19:00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Working on making generalized code which should work for all three files. </t>
   </si>
 </sst>
 </file>
@@ -1003,10 +1051,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07624C4B-536F-4CB7-AB8E-70C51D83A0BA}">
-  <dimension ref="A1:C100"/>
+  <dimension ref="A1:C110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
-      <selection activeCell="C101" sqref="C101"/>
+    <sheetView tabSelected="1" topLeftCell="A97" workbookViewId="0">
+      <selection activeCell="D110" sqref="D110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2062,6 +2110,110 @@
         <v>8</v>
       </c>
     </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A101" s="5"/>
+      <c r="B101" s="6"/>
+      <c r="C101" s="5"/>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A102" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="B102" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="C102" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A103" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="B103" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="C103" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A104" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="B104" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="C104" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A105" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="B105" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="C105" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A106" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="B106" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C106" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A107" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="B107" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="C107" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A108" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="B108" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="C108" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A109" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="B109" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="C109" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A110" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="B110" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="C110" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added timesheet of date 12-02-2020
</commit_message>
<xml_diff>
--- a/Timesheet January 2020.xlsx
+++ b/Timesheet January 2020.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\Timesheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A33B0EA9-F709-43BE-9729-ABF3A3F4981E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3C78E82-434B-46DE-9B68-F6FD1A00C23E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{4E06B61D-CC95-4C6D-96A7-14002220E881}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="215">
   <si>
     <t>Timestamp</t>
   </si>
@@ -661,6 +661,70 @@
   </si>
   <si>
     <t xml:space="preserve">Working on making generalized code which should work for all three files. </t>
+  </si>
+  <si>
+    <t>Feb 12 10:00 to 11:00</t>
+  </si>
+  <si>
+    <t>Generalized code for hourly bucket creation, now code is working for both system and
+event file. Combined both data using full outer join.</t>
+  </si>
+  <si>
+    <t>Feb 12 11:00 to 12:00</t>
+  </si>
+  <si>
+    <t>Worked on progress bar, no progress bar startegy working. Working on other progress
+bar strategy.</t>
+  </si>
+  <si>
+    <t>Feb 12 12:00 to 13:00</t>
+  </si>
+  <si>
+    <t>Progress bar done for labelling hourly buckets and making bucket data. Modifying code
+to make it totally object oriented.</t>
+  </si>
+  <si>
+    <t>Feb 12 13:00 to 13:30</t>
+  </si>
+  <si>
+    <t>Creating folder for properly storing data files. Making it machine wise.</t>
+  </si>
+  <si>
+    <t>Feb 12 13:30 to 14:30</t>
+  </si>
+  <si>
+    <t>Feb 12 14:30 to 15:00</t>
+  </si>
+  <si>
+    <t>Modified code for progress bar</t>
+  </si>
+  <si>
+    <t>Feb 12 15:00 to 16:00</t>
+  </si>
+  <si>
+    <t>Added code for combining machine wise data</t>
+  </si>
+  <si>
+    <t>Feb 12 16:00 to 17:00</t>
+  </si>
+  <si>
+    <t>Office trip</t>
+  </si>
+  <si>
+    <t>Code modified for combining hourly data of machines.</t>
+  </si>
+  <si>
+    <t>Feb 12 17:00 to 18:30</t>
+  </si>
+  <si>
+    <t>Chatrapati chowk,
+Pratap Nagar.</t>
+  </si>
+  <si>
+    <t>Feb 12 18:30 to 19:00</t>
+  </si>
+  <si>
+    <t>Saved combined data by creating separate folder.</t>
   </si>
 </sst>
 </file>
@@ -708,7 +772,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -736,6 +800,9 @@
     </xf>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1051,10 +1118,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07624C4B-536F-4CB7-AB8E-70C51D83A0BA}">
-  <dimension ref="A1:C110"/>
+  <dimension ref="A1:C121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A97" workbookViewId="0">
-      <selection activeCell="D110" sqref="D110"/>
+    <sheetView tabSelected="1" topLeftCell="A107" workbookViewId="0">
+      <selection activeCell="C122" sqref="C122"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2214,6 +2281,121 @@
         <v>8</v>
       </c>
     </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A111" s="5"/>
+      <c r="B111" s="6"/>
+      <c r="C111" s="5"/>
+    </row>
+    <row r="112" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A112" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="B112" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="C112" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A113" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="B113" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="C113" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A114" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="B114" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="C114" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A115" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="B115" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="C115" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A116" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="B116" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C116" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A117" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="B117" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="C117" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A118" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="B118" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="C118" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A119" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="B119" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="C119" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A120" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="B120" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="C120" s="10" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A121" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="B121" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="C121" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added timesheet of date 14-02-2020
</commit_message>
<xml_diff>
--- a/Timesheet January 2020.xlsx
+++ b/Timesheet January 2020.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\Timesheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3C78E82-434B-46DE-9B68-F6FD1A00C23E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{553D65A0-2D83-442F-8DA1-A00C45903BC3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{4E06B61D-CC95-4C6D-96A7-14002220E881}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="246">
   <si>
     <t>Timestamp</t>
   </si>
@@ -725,16 +725,118 @@
   </si>
   <si>
     <t>Saved combined data by creating separate folder.</t>
+  </si>
+  <si>
+    <t>Feb 13 10:00 to 11:00</t>
+  </si>
+  <si>
+    <t>Saved combined data. Modified code for creating combined data. Doing analysis of
+combined data on jupyter notebook.</t>
+  </si>
+  <si>
+    <t>Feb 13 11:00 to 12:00</t>
+  </si>
+  <si>
+    <t>Cleaned combined data and finding lags between start and end date.</t>
+  </si>
+  <si>
+    <t>Feb 13 12:00 to 13:00</t>
+  </si>
+  <si>
+    <t>Documented observations and conclusion.</t>
+  </si>
+  <si>
+    <t>Feb 13 13:00 to 14:00</t>
+  </si>
+  <si>
+    <t>Feb 13 14:00 to 15:00</t>
+  </si>
+  <si>
+    <t>Modified code of hourly data making, got error. Working on resolving erros.</t>
+  </si>
+  <si>
+    <t>Feb 13 15:00 to 16:00</t>
+  </si>
+  <si>
+    <t>Python Class, made the code as it was earlier.</t>
+  </si>
+  <si>
+    <t>Feb 13 16:00 to 17:00</t>
+  </si>
+  <si>
+    <t>Understanding python decorator and metaprogramming.</t>
+  </si>
+  <si>
+    <t>Feb 13 17:00 to 18:00</t>
+  </si>
+  <si>
+    <t>Understanding python method overloading and method overriding.</t>
+  </si>
+  <si>
+    <t>Feb 13 18:00 to 19:00</t>
+  </si>
+  <si>
+    <t>requirement analysis of model building for dashscope project.</t>
+  </si>
+  <si>
+    <t>Feb 14 10:00 to 11:00</t>
+  </si>
+  <si>
+    <t>Understood ML pipeline. Viewed a example of ML pipeline in python. Figured out steps
+for building ML pipeline for PAM data exploration. Added pictorial representation in 
+presentation file.</t>
+  </si>
+  <si>
+    <t>Feb 14 11:00 to 12:00</t>
+  </si>
+  <si>
+    <t>Making separate ML pipeline directory.</t>
+  </si>
+  <si>
+    <t>Feb 14 12:00 to 13:00</t>
+  </si>
+  <si>
+    <t>Added code to ML pipeline directory, made separate virtual environment.</t>
+  </si>
+  <si>
+    <t>Feb 14 13:00 to 14:00</t>
+  </si>
+  <si>
+    <t>Feb 14 14:00 to 17:30</t>
+  </si>
+  <si>
+    <t>SIA, went to MR students school.</t>
+  </si>
+  <si>
+    <t>Jawahar nagar, Manewada</t>
+  </si>
+  <si>
+    <t>Feb 14 17:30 to 18:00</t>
+  </si>
+  <si>
+    <t>Worked on data cleaning.</t>
+  </si>
+  <si>
+    <t>Feb 14 18:00 to 19:00</t>
+  </si>
+  <si>
+    <t>Got problems while implementing data cleaning using OOP concepts.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -772,7 +874,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -803,6 +905,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1118,17 +1226,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07624C4B-536F-4CB7-AB8E-70C51D83A0BA}">
-  <dimension ref="A1:C121"/>
+  <dimension ref="A1:C139"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A107" workbookViewId="0">
-      <selection activeCell="C122" sqref="C122"/>
+    <sheetView tabSelected="1" topLeftCell="A119" workbookViewId="0">
+      <selection activeCell="C140" sqref="C140"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="25.85546875" style="1" customWidth="1"/>
     <col min="2" max="2" width="79.42578125" style="3" customWidth="1"/>
-    <col min="3" max="3" width="22.5703125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="34.42578125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -2396,7 +2504,194 @@
         <v>8</v>
       </c>
     </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A122" s="11"/>
+      <c r="B122" s="12"/>
+      <c r="C122" s="11"/>
+    </row>
+    <row r="123" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A123" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="B123" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="C123" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A124" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="B124" s="3" t="s">
+        <v>218</v>
+      </c>
+      <c r="C124" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A125" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="B125" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="C125" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A126" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="B126" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C126" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A127" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="B127" s="3" t="s">
+        <v>223</v>
+      </c>
+      <c r="C127" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A128" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="B128" s="3" t="s">
+        <v>225</v>
+      </c>
+      <c r="C128" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A129" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="B129" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="C129" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A130" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="B130" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="C130" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A131" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="B131" s="3" t="s">
+        <v>231</v>
+      </c>
+      <c r="C131" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A132" s="5"/>
+      <c r="B132" s="6"/>
+      <c r="C132" s="5"/>
+    </row>
+    <row r="133" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A133" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="B133" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="C133" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A134" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="B134" s="3" t="s">
+        <v>235</v>
+      </c>
+      <c r="C134" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A135" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="B135" s="3" t="s">
+        <v>237</v>
+      </c>
+      <c r="C135" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A136" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="B136" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C136" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A137" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="B137" s="3" t="s">
+        <v>240</v>
+      </c>
+      <c r="C137" s="1" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A138" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="B138" s="3" t="s">
+        <v>243</v>
+      </c>
+      <c r="C138" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A139" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="B139" s="3" t="s">
+        <v>245</v>
+      </c>
+      <c r="C139" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added timesheet of date 17-02-2020
</commit_message>
<xml_diff>
--- a/Timesheet January 2020.xlsx
+++ b/Timesheet January 2020.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\Timesheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{553D65A0-2D83-442F-8DA1-A00C45903BC3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51CA67CB-717F-42B4-92B9-7C67D3C8C558}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{4E06B61D-CC95-4C6D-96A7-14002220E881}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="246">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="265">
   <si>
     <t>Timestamp</t>
   </si>
@@ -821,6 +821,66 @@
   </si>
   <si>
     <t>Got problems while implementing data cleaning using OOP concepts.</t>
+  </si>
+  <si>
+    <t>Feb 17 10:00 to 11:00</t>
+  </si>
+  <si>
+    <t>Modified code of hourly data buckets, added combined data check</t>
+  </si>
+  <si>
+    <t>Feb 17 11:00 to 12:00</t>
+  </si>
+  <si>
+    <t>Documenting and commenting HourWiseData class</t>
+  </si>
+  <si>
+    <t>Feb 17 12:00 to 13:00</t>
+  </si>
+  <si>
+    <t>Documented and commented HourWiseData class. Documenting and commenting
+HourlyMachineData class</t>
+  </si>
+  <si>
+    <t>Feb 17 13:00 to 13:30</t>
+  </si>
+  <si>
+    <t>Documented and commented HourlyMachineData class.</t>
+  </si>
+  <si>
+    <t>Feb 17 13:30 to 14:00</t>
+  </si>
+  <si>
+    <t>Feb 17 14:00 to 15:00</t>
+  </si>
+  <si>
+    <t>Data Cleaning done. Working on data transformation.</t>
+  </si>
+  <si>
+    <t>Feb 17 15:00 to 16:00</t>
+  </si>
+  <si>
+    <t>Getting errors and complication in data transformation. Working on fixing issues</t>
+  </si>
+  <si>
+    <t>Feb 17 16:00 to 17:00</t>
+  </si>
+  <si>
+    <t>Not considering data transformation due to issues in loading saved combined data.
+Removed code of saving combined data.</t>
+  </si>
+  <si>
+    <t>Feb 17 17:00 to 18:00</t>
+  </si>
+  <si>
+    <t>Worked on feature engineering. Created features as max occurred sublocation, total
+alarm duration and total automation duration.</t>
+  </si>
+  <si>
+    <t>Feb 17 18:00 to 19:00</t>
+  </si>
+  <si>
+    <t>Getting issues and complications in feature engineering progress bars.</t>
   </si>
 </sst>
 </file>
@@ -1226,10 +1286,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07624C4B-536F-4CB7-AB8E-70C51D83A0BA}">
-  <dimension ref="A1:C139"/>
+  <dimension ref="A1:C150"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A119" workbookViewId="0">
-      <selection activeCell="C140" sqref="C140"/>
+    <sheetView tabSelected="1" topLeftCell="A134" workbookViewId="0">
+      <selection activeCell="D150" sqref="D150"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2690,6 +2750,121 @@
         <v>8</v>
       </c>
     </row>
+    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A140" s="5"/>
+      <c r="B140" s="6"/>
+      <c r="C140" s="5"/>
+    </row>
+    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A141" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="B141" s="3" t="s">
+        <v>247</v>
+      </c>
+      <c r="C141" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A142" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="B142" s="3" t="s">
+        <v>249</v>
+      </c>
+      <c r="C142" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A143" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="B143" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="C143" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A144" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="B144" s="3" t="s">
+        <v>253</v>
+      </c>
+      <c r="C144" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A145" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="B145" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C145" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A146" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="B146" s="3" t="s">
+        <v>256</v>
+      </c>
+      <c r="C146" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A147" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="B147" s="3" t="s">
+        <v>258</v>
+      </c>
+      <c r="C147" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="148" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A148" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="B148" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="C148" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="149" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A149" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="B149" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="C149" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="150" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A150" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="B150" s="3" t="s">
+        <v>264</v>
+      </c>
+      <c r="C150" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Added timesheet of date 18-02-2020
</commit_message>
<xml_diff>
--- a/Timesheet January 2020.xlsx
+++ b/Timesheet January 2020.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\Timesheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51CA67CB-717F-42B4-92B9-7C67D3C8C558}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA807AB6-407E-4F99-8B10-47E536D3E6F4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{4E06B61D-CC95-4C6D-96A7-14002220E881}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="265">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="284">
   <si>
     <t>Timestamp</t>
   </si>
@@ -881,6 +881,64 @@
   </si>
   <si>
     <t>Getting issues and complications in feature engineering progress bars.</t>
+  </si>
+  <si>
+    <t>Feb 18 10:00 to 11:00</t>
+  </si>
+  <si>
+    <t>Documented feature engineering code</t>
+  </si>
+  <si>
+    <t>Feb 18 11:00 to 12:00</t>
+  </si>
+  <si>
+    <t>Documented data cleaning and app code</t>
+  </si>
+  <si>
+    <t>Feb 18 12:00 to 13:00</t>
+  </si>
+  <si>
+    <t>worked on separate console message functionality, droped idea due to inconvinience
+in class decoration.</t>
+  </si>
+  <si>
+    <t>Feb 18 13:00 to 13:30</t>
+  </si>
+  <si>
+    <t>Working on data transformation, logic is little complicated</t>
+  </si>
+  <si>
+    <t>Feb 18 13:30 to 14:00</t>
+  </si>
+  <si>
+    <t>Feb 18 14:00 to 15:00</t>
+  </si>
+  <si>
+    <t>Worked on data transformation, getting errors in process.</t>
+  </si>
+  <si>
+    <t>Feb 18 15:00 to 16:00</t>
+  </si>
+  <si>
+    <t>Logic failed for data transformation, using pycharm for debugging project</t>
+  </si>
+  <si>
+    <t>Feb 18 16:00 to 17:00</t>
+  </si>
+  <si>
+    <t>Modified some code for data transformation, data transformation working.</t>
+  </si>
+  <si>
+    <t>Feb 18 17:00 to 18:00</t>
+  </si>
+  <si>
+    <t>Modified code of progress bar, progress bars are working.</t>
+  </si>
+  <si>
+    <t>Feb 18 18:00 to 19:00</t>
+  </si>
+  <si>
+    <t>Created new features.</t>
   </si>
 </sst>
 </file>
@@ -1286,10 +1344,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07624C4B-536F-4CB7-AB8E-70C51D83A0BA}">
-  <dimension ref="A1:C150"/>
+  <dimension ref="A1:C161"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A134" workbookViewId="0">
-      <selection activeCell="D150" sqref="D150"/>
+    <sheetView tabSelected="1" topLeftCell="A143" workbookViewId="0">
+      <selection activeCell="D161" sqref="D161"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2865,6 +2923,121 @@
         <v>8</v>
       </c>
     </row>
+    <row r="151" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A151" s="5"/>
+      <c r="B151" s="6"/>
+      <c r="C151" s="5"/>
+    </row>
+    <row r="152" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A152" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="B152" s="3" t="s">
+        <v>266</v>
+      </c>
+      <c r="C152" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="153" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A153" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="B153" s="3" t="s">
+        <v>268</v>
+      </c>
+      <c r="C153" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="154" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A154" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="B154" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="C154" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="155" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A155" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="B155" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="C155" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="156" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A156" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="B156" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C156" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="157" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A157" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="B157" s="3" t="s">
+        <v>275</v>
+      </c>
+      <c r="C157" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="158" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A158" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="B158" s="3" t="s">
+        <v>277</v>
+      </c>
+      <c r="C158" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="159" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A159" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="B159" s="3" t="s">
+        <v>279</v>
+      </c>
+      <c r="C159" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="160" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A160" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="B160" s="3" t="s">
+        <v>281</v>
+      </c>
+      <c r="C160" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="161" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A161" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="B161" s="3" t="s">
+        <v>283</v>
+      </c>
+      <c r="C161" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Added timesheet of date 19-02-2020
</commit_message>
<xml_diff>
--- a/Timesheet January 2020.xlsx
+++ b/Timesheet January 2020.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\Timesheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA807AB6-407E-4F99-8B10-47E536D3E6F4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{827B8CB0-B445-4F93-A30F-4BCC239B28E8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{4E06B61D-CC95-4C6D-96A7-14002220E881}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="284">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="465" uniqueCount="301">
   <si>
     <t>Timestamp</t>
   </si>
@@ -939,6 +939,59 @@
   </si>
   <si>
     <t>Created new features.</t>
+  </si>
+  <si>
+    <t>Feb 19 10:00 to 11:00</t>
+  </si>
+  <si>
+    <t>Saved transformed data, used json configuration file, but logic did not worked. Saved
+using declaring path in class.</t>
+  </si>
+  <si>
+    <t>Feb 19 11:00 to 12:00</t>
+  </si>
+  <si>
+    <t>Documenting code properly</t>
+  </si>
+  <si>
+    <t>Feb 19 12:00 to 13:00</t>
+  </si>
+  <si>
+    <t>Feb 19 13:00 to 14:00</t>
+  </si>
+  <si>
+    <t>Documented and commented data transformation</t>
+  </si>
+  <si>
+    <t>Worked on code generator problem</t>
+  </si>
+  <si>
+    <t>Feb 19 14:00 to 15:00</t>
+  </si>
+  <si>
+    <t>Feb 19 15:00 to 16:00</t>
+  </si>
+  <si>
+    <t>Started statistical analysis phase of ml pipeline. Created new jupyter notebook</t>
+  </si>
+  <si>
+    <t>Feb 19 16:00 to 17:00</t>
+  </si>
+  <si>
+    <t>Checking null values</t>
+  </si>
+  <si>
+    <t>Feb 19 17:00 to 18:00</t>
+  </si>
+  <si>
+    <t>Printing total null values of both data. Displayed descriptive statistic of selected columns</t>
+  </si>
+  <si>
+    <t>Feb 19 18:00 to 19:00</t>
+  </si>
+  <si>
+    <t>Identified outliers in alarm and automation duration. Working on outlier removal, lag
+detections and statistical hypothesis testing.</t>
   </si>
 </sst>
 </file>
@@ -1344,10 +1397,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07624C4B-536F-4CB7-AB8E-70C51D83A0BA}">
-  <dimension ref="A1:C161"/>
+  <dimension ref="A1:C171"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A143" workbookViewId="0">
-      <selection activeCell="D161" sqref="D161"/>
+    <sheetView tabSelected="1" topLeftCell="A157" workbookViewId="0">
+      <selection activeCell="D171" sqref="D171"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3038,6 +3091,110 @@
         <v>8</v>
       </c>
     </row>
+    <row r="162" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A162" s="5"/>
+      <c r="B162" s="6"/>
+      <c r="C162" s="5"/>
+    </row>
+    <row r="163" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A163" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="B163" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="C163" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="164" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A164" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="B164" s="3" t="s">
+        <v>287</v>
+      </c>
+      <c r="C164" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="165" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A165" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="B165" s="3" t="s">
+        <v>290</v>
+      </c>
+      <c r="C165" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="166" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A166" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="B166" s="3" t="s">
+        <v>291</v>
+      </c>
+      <c r="C166" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="167" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A167" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="B167" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C167" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="168" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A168" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="B168" s="3" t="s">
+        <v>294</v>
+      </c>
+      <c r="C168" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="169" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A169" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="B169" s="3" t="s">
+        <v>296</v>
+      </c>
+      <c r="C169" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="170" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A170" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="B170" s="3" t="s">
+        <v>298</v>
+      </c>
+      <c r="C170" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="171" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A171" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="B171" s="2" t="s">
+        <v>300</v>
+      </c>
+      <c r="C171" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Added timesheet of date 20-02-2020
</commit_message>
<xml_diff>
--- a/Timesheet January 2020.xlsx
+++ b/Timesheet January 2020.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\Timesheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{827B8CB0-B445-4F93-A30F-4BCC239B28E8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0988E89-FCE9-4B38-854F-FD1404862500}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{4E06B61D-CC95-4C6D-96A7-14002220E881}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="465" uniqueCount="301">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="495" uniqueCount="320">
   <si>
     <t>Timestamp</t>
   </si>
@@ -992,6 +992,64 @@
   <si>
     <t>Identified outliers in alarm and automation duration. Working on outlier removal, lag
 detections and statistical hypothesis testing.</t>
+  </si>
+  <si>
+    <t>Feb 20 10:00 to 11:00</t>
+  </si>
+  <si>
+    <t>Removed outliers from data, modified some of the code.</t>
+  </si>
+  <si>
+    <t>Feb 20 11:00 to 12:00</t>
+  </si>
+  <si>
+    <t>Found lags in data</t>
+  </si>
+  <si>
+    <t>Feb 20 12:00 to 13:00</t>
+  </si>
+  <si>
+    <t>Removed lags from data</t>
+  </si>
+  <si>
+    <t>Feb 20 13:00 to 13:30</t>
+  </si>
+  <si>
+    <t>Ploted trend, looking for other methods to plot trend.</t>
+  </si>
+  <si>
+    <t>Feb 20 13:30 to 14:30</t>
+  </si>
+  <si>
+    <t>Feb 20 14:30 to 15:00</t>
+  </si>
+  <si>
+    <t>Concatinated data</t>
+  </si>
+  <si>
+    <t>Feb 20 15:00 to 16:00</t>
+  </si>
+  <si>
+    <t>Created new feature hour, dropped hourly timestamp. Started model building</t>
+  </si>
+  <si>
+    <t>Feb 20 16:00 to 17:00</t>
+  </si>
+  <si>
+    <t>Model builded, applied linear regresion</t>
+  </si>
+  <si>
+    <t>Feb 20 17:00 to 18:00</t>
+  </si>
+  <si>
+    <t>Checked accuracy of model</t>
+  </si>
+  <si>
+    <t>Feb 20 18:00 to 19:00</t>
+  </si>
+  <si>
+    <t>Modified code, made separate modules inside ML pipeline package, working on multiple
+model processing.</t>
   </si>
 </sst>
 </file>
@@ -1397,10 +1455,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07624C4B-536F-4CB7-AB8E-70C51D83A0BA}">
-  <dimension ref="A1:C171"/>
+  <dimension ref="A1:C182"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A157" workbookViewId="0">
-      <selection activeCell="D171" sqref="D171"/>
+    <sheetView tabSelected="1" topLeftCell="A158" workbookViewId="0">
+      <selection activeCell="D182" sqref="D182"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3195,6 +3253,121 @@
         <v>8</v>
       </c>
     </row>
+    <row r="172" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A172" s="5"/>
+      <c r="B172" s="6"/>
+      <c r="C172" s="5"/>
+    </row>
+    <row r="173" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A173" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="B173" s="3" t="s">
+        <v>302</v>
+      </c>
+      <c r="C173" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="174" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A174" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="B174" s="3" t="s">
+        <v>304</v>
+      </c>
+      <c r="C174" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="175" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A175" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="B175" s="3" t="s">
+        <v>306</v>
+      </c>
+      <c r="C175" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="176" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A176" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="B176" s="3" t="s">
+        <v>308</v>
+      </c>
+      <c r="C176" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="177" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A177" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="B177" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C177" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="178" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A178" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="B178" s="3" t="s">
+        <v>311</v>
+      </c>
+      <c r="C178" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="179" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A179" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="B179" s="3" t="s">
+        <v>313</v>
+      </c>
+      <c r="C179" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="180" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A180" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="B180" s="3" t="s">
+        <v>315</v>
+      </c>
+      <c r="C180" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="181" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A181" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="B181" s="3" t="s">
+        <v>317</v>
+      </c>
+      <c r="C181" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="182" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A182" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="B182" s="2" t="s">
+        <v>319</v>
+      </c>
+      <c r="C182" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Added timesheet and disscusion of date 21-02-2020
</commit_message>
<xml_diff>
--- a/Timesheet January 2020.xlsx
+++ b/Timesheet January 2020.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\Timesheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0988E89-FCE9-4B38-854F-FD1404862500}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B43E030-5C66-43CA-9C21-D4F08116C4EC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{4E06B61D-CC95-4C6D-96A7-14002220E881}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="495" uniqueCount="320">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="516" uniqueCount="333">
   <si>
     <t>Timestamp</t>
   </si>
@@ -1050,6 +1050,47 @@
   <si>
     <t>Modified code, made separate modules inside ML pipeline package, working on multiple
 model processing.</t>
+  </si>
+  <si>
+    <t>Builded Decision tree, random forest, support vector machine and k-nearest neighbour
+models and compared there accuracy.</t>
+  </si>
+  <si>
+    <t>Builded multilayer perceptron model, modified some code. Working on model tuning</t>
+  </si>
+  <si>
+    <t>Sapphire auomation</t>
+  </si>
+  <si>
+    <t>Feb 21 13:00 to 14:00</t>
+  </si>
+  <si>
+    <t>Practiced some examples of django based deployement of ml models</t>
+  </si>
+  <si>
+    <t>Feb 21 12:00 to 13:00</t>
+  </si>
+  <si>
+    <t>Feb 21 11:00 to 12:00</t>
+  </si>
+  <si>
+    <t>Feb 21 10:00 to 11:00</t>
+  </si>
+  <si>
+    <t>Feb 21 14:00 to 15:00</t>
+  </si>
+  <si>
+    <t>Feb 21 15:00 to 16:00</t>
+  </si>
+  <si>
+    <t>Modified code. Added code which save model as pickled model</t>
+  </si>
+  <si>
+    <t>Feb 21 16:00 to 19:00</t>
+  </si>
+  <si>
+    <t>Worked on many django based ml model deployement examples, none were executed
+successfully.</t>
   </si>
 </sst>
 </file>
@@ -1455,10 +1496,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07624C4B-536F-4CB7-AB8E-70C51D83A0BA}">
-  <dimension ref="A1:C182"/>
+  <dimension ref="A1:C190"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A158" workbookViewId="0">
-      <selection activeCell="D182" sqref="D182"/>
+    <sheetView tabSelected="1" topLeftCell="A179" workbookViewId="0">
+      <selection activeCell="D190" sqref="D190"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3368,6 +3409,88 @@
         <v>8</v>
       </c>
     </row>
+    <row r="183" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A183" s="5"/>
+      <c r="B183" s="6"/>
+      <c r="C183" s="5"/>
+    </row>
+    <row r="184" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A184" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="B184" s="2" t="s">
+        <v>320</v>
+      </c>
+      <c r="C184" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="185" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A185" s="1" t="s">
+        <v>326</v>
+      </c>
+      <c r="B185" s="3" t="s">
+        <v>321</v>
+      </c>
+      <c r="C185" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="186" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A186" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="B186" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C186" s="1" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="187" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A187" s="1" t="s">
+        <v>323</v>
+      </c>
+      <c r="B187" s="3" t="s">
+        <v>324</v>
+      </c>
+      <c r="C187" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="188" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A188" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="B188" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C188" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="189" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A189" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="B189" s="3" t="s">
+        <v>330</v>
+      </c>
+      <c r="C189" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="190" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A190" s="1" t="s">
+        <v>331</v>
+      </c>
+      <c r="B190" s="2" t="s">
+        <v>332</v>
+      </c>
+      <c r="C190" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Added timesheet of date 25-02-2020
</commit_message>
<xml_diff>
--- a/Timesheet January 2020.xlsx
+++ b/Timesheet January 2020.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\Timesheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B43E030-5C66-43CA-9C21-D4F08116C4EC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD5036FB-C585-4837-9F5B-E09C83D0C457}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{4E06B61D-CC95-4C6D-96A7-14002220E881}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="516" uniqueCount="333">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="564" uniqueCount="364">
   <si>
     <t>Timestamp</t>
   </si>
@@ -1091,6 +1091,100 @@
   <si>
     <t>Worked on many django based ml model deployement examples, none were executed
 successfully.</t>
+  </si>
+  <si>
+    <t>Feb 24 10:00 to 11:00</t>
+  </si>
+  <si>
+    <t>Build django backend. Predictions are fetched.</t>
+  </si>
+  <si>
+    <t>Feb 24 11:00 to 12:00</t>
+  </si>
+  <si>
+    <t>Modified some code of ml phases. Making some features in django backend.</t>
+  </si>
+  <si>
+    <t>Feb 24 12:00 to 13:00</t>
+  </si>
+  <si>
+    <t>Modified some code of ml phases.</t>
+  </si>
+  <si>
+    <t>Feb 24 13:00 to 14:00</t>
+  </si>
+  <si>
+    <t>Feb 24 14:00 to 17:36</t>
+  </si>
+  <si>
+    <t>Embros technology</t>
+  </si>
+  <si>
+    <t>Chatrapati chowk</t>
+  </si>
+  <si>
+    <t>Feb 24 17:36 to 18:00</t>
+  </si>
+  <si>
+    <t>Modified django backend code, got error, working on code.</t>
+  </si>
+  <si>
+    <t>Feb 25 10:00 to 11:00</t>
+  </si>
+  <si>
+    <t>Used HTTP PATCH method for sending multiple data to api server. Found 60-total alarm
+time + error relationship of sample predictive model.</t>
+  </si>
+  <si>
+    <t>Feb 25 11:00 to 12:00</t>
+  </si>
+  <si>
+    <t>Working on integrating ml code in backend.</t>
+  </si>
+  <si>
+    <t>Feb 25 12:00 to 13:00</t>
+  </si>
+  <si>
+    <t>Created uml of data files</t>
+  </si>
+  <si>
+    <t>Feb 25 13:00 to 13:30</t>
+  </si>
+  <si>
+    <t>Feb 25 13:30 to 14:00</t>
+  </si>
+  <si>
+    <t>Created uml for combined data</t>
+  </si>
+  <si>
+    <t>Feb 25 14:00 to 15:00</t>
+  </si>
+  <si>
+    <t>Tried to upload Djangomlapi to heroku, app was not uploaded but not worked.</t>
+  </si>
+  <si>
+    <t>Feb 25 15:00 to 16:00</t>
+  </si>
+  <si>
+    <t>Making a normal api with django api</t>
+  </si>
+  <si>
+    <t>Feb 25 16:00 to 17:00</t>
+  </si>
+  <si>
+    <t>Made a normal api using views only, data sent to post gets lost, working on issue</t>
+  </si>
+  <si>
+    <t>Feb 25 17:00 to 18:00</t>
+  </si>
+  <si>
+    <t>working on multivariate timeseries algo.</t>
+  </si>
+  <si>
+    <t>Feb 25 18:00 to 19:00</t>
+  </si>
+  <si>
+    <t>Worked on MVTA, tyring some exaples.</t>
   </si>
 </sst>
 </file>
@@ -1496,10 +1590,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07624C4B-536F-4CB7-AB8E-70C51D83A0BA}">
-  <dimension ref="A1:C190"/>
+  <dimension ref="A1:C208"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A179" workbookViewId="0">
-      <selection activeCell="D190" sqref="D190"/>
+    <sheetView tabSelected="1" topLeftCell="A192" workbookViewId="0">
+      <selection activeCell="A209" sqref="A209"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3491,6 +3585,192 @@
         <v>8</v>
       </c>
     </row>
+    <row r="191" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A191" s="5"/>
+      <c r="B191" s="6"/>
+      <c r="C191" s="5"/>
+    </row>
+    <row r="192" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A192" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="B192" s="3" t="s">
+        <v>334</v>
+      </c>
+      <c r="C192" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="193" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A193" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="B193" s="3" t="s">
+        <v>336</v>
+      </c>
+      <c r="C193" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="194" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A194" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="B194" s="3" t="s">
+        <v>338</v>
+      </c>
+      <c r="C194" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="195" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A195" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="B195" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C195" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="196" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A196" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="B196" s="3" t="s">
+        <v>341</v>
+      </c>
+      <c r="C196" s="1" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="197" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A197" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="B197" s="3" t="s">
+        <v>344</v>
+      </c>
+      <c r="C197" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="198" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A198" s="5"/>
+      <c r="B198" s="6"/>
+      <c r="C198" s="5"/>
+    </row>
+    <row r="199" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A199" s="1" t="s">
+        <v>345</v>
+      </c>
+      <c r="B199" s="2" t="s">
+        <v>346</v>
+      </c>
+      <c r="C199" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="200" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A200" s="1" t="s">
+        <v>347</v>
+      </c>
+      <c r="B200" s="3" t="s">
+        <v>348</v>
+      </c>
+      <c r="C200" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="201" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A201" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="B201" s="3" t="s">
+        <v>350</v>
+      </c>
+      <c r="C201" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="202" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A202" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="B202" s="3" t="s">
+        <v>353</v>
+      </c>
+      <c r="C202" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="203" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A203" s="1" t="s">
+        <v>352</v>
+      </c>
+      <c r="B203" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C203" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="204" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A204" s="1" t="s">
+        <v>354</v>
+      </c>
+      <c r="B204" s="3" t="s">
+        <v>355</v>
+      </c>
+      <c r="C204" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="205" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A205" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="B205" s="3" t="s">
+        <v>357</v>
+      </c>
+      <c r="C205" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="206" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A206" s="1" t="s">
+        <v>358</v>
+      </c>
+      <c r="B206" s="3" t="s">
+        <v>359</v>
+      </c>
+      <c r="C206" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="207" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A207" s="1" t="s">
+        <v>360</v>
+      </c>
+      <c r="B207" s="3" t="s">
+        <v>361</v>
+      </c>
+      <c r="C207" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="208" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A208" s="1" t="s">
+        <v>362</v>
+      </c>
+      <c r="B208" s="3" t="s">
+        <v>363</v>
+      </c>
+      <c r="C208" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Added timesheet of date 26-02-2020
</commit_message>
<xml_diff>
--- a/Timesheet January 2020.xlsx
+++ b/Timesheet January 2020.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\Timesheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD5036FB-C585-4837-9F5B-E09C83D0C457}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68D15033-DA20-4364-BFBF-7F2F28239611}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{4E06B61D-CC95-4C6D-96A7-14002220E881}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="564" uniqueCount="364">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="591" uniqueCount="381">
   <si>
     <t>Timestamp</t>
   </si>
@@ -1185,6 +1185,59 @@
   </si>
   <si>
     <t>Worked on MVTA, tyring some exaples.</t>
+  </si>
+  <si>
+    <t>Performing multi variate timeseries on combined horly data, done upto making date
+time index.</t>
+  </si>
+  <si>
+    <t>Build Multivariate timeseries model using var algo. Got problem in label decoding.
+Results were not good. Working on sample UI page.</t>
+  </si>
+  <si>
+    <t>made wireframe of sample UI</t>
+  </si>
+  <si>
+    <t>viewd some django documentation</t>
+  </si>
+  <si>
+    <t>Feb 26 10:00 to 11:00</t>
+  </si>
+  <si>
+    <t>Feb 26 11:00 to 12:00</t>
+  </si>
+  <si>
+    <t>Feb 26 12:00 to 13:00</t>
+  </si>
+  <si>
+    <t>Feb 26 13:00 to 13:30</t>
+  </si>
+  <si>
+    <t>Feb 26 13:30 to 14:00</t>
+  </si>
+  <si>
+    <t>Feb 26 14:00 to 15:00</t>
+  </si>
+  <si>
+    <t>Working on rest api</t>
+  </si>
+  <si>
+    <t>Feb 26 15:00 to 16:00</t>
+  </si>
+  <si>
+    <t>Made a sample django api with rest, used post for json sucessfully</t>
+  </si>
+  <si>
+    <t>Feb 26 16:00 to 17:00</t>
+  </si>
+  <si>
+    <t>Made sample django app which accepts initials of name and return full name</t>
+  </si>
+  <si>
+    <t>Feb 26 17:00 to 20:00</t>
+  </si>
+  <si>
+    <t>Did a example considering up time, output count and harmful alarms</t>
   </si>
 </sst>
 </file>
@@ -1590,10 +1643,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07624C4B-536F-4CB7-AB8E-70C51D83A0BA}">
-  <dimension ref="A1:C208"/>
+  <dimension ref="A1:C218"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A192" workbookViewId="0">
-      <selection activeCell="A209" sqref="A209"/>
+    <sheetView tabSelected="1" topLeftCell="A195" workbookViewId="0">
+      <selection activeCell="D218" sqref="D218"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3771,6 +3824,110 @@
         <v>8</v>
       </c>
     </row>
+    <row r="209" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A209" s="5"/>
+      <c r="B209" s="6"/>
+      <c r="C209" s="5"/>
+    </row>
+    <row r="210" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A210" s="1" t="s">
+        <v>368</v>
+      </c>
+      <c r="B210" s="2" t="s">
+        <v>364</v>
+      </c>
+      <c r="C210" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="211" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A211" s="1" t="s">
+        <v>369</v>
+      </c>
+      <c r="B211" s="2" t="s">
+        <v>365</v>
+      </c>
+      <c r="C211" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="212" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A212" s="1" t="s">
+        <v>370</v>
+      </c>
+      <c r="B212" s="3" t="s">
+        <v>366</v>
+      </c>
+      <c r="C212" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="213" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A213" s="1" t="s">
+        <v>371</v>
+      </c>
+      <c r="B213" s="3" t="s">
+        <v>367</v>
+      </c>
+      <c r="C213" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="214" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A214" s="9" t="s">
+        <v>372</v>
+      </c>
+      <c r="B214" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C214" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="215" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A215" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="B215" s="3" t="s">
+        <v>374</v>
+      </c>
+      <c r="C215" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="216" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A216" s="1" t="s">
+        <v>375</v>
+      </c>
+      <c r="B216" s="3" t="s">
+        <v>376</v>
+      </c>
+      <c r="C216" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="217" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A217" s="1" t="s">
+        <v>377</v>
+      </c>
+      <c r="B217" s="3" t="s">
+        <v>378</v>
+      </c>
+      <c r="C217" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="218" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A218" s="1" t="s">
+        <v>379</v>
+      </c>
+      <c r="B218" s="3" t="s">
+        <v>380</v>
+      </c>
+      <c r="C218" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Added timesheet of date 27-02-2020
</commit_message>
<xml_diff>
--- a/Timesheet January 2020.xlsx
+++ b/Timesheet January 2020.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\Timesheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68D15033-DA20-4364-BFBF-7F2F28239611}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44121EF9-DB72-4F1E-A8A5-548DFB04472C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{4E06B61D-CC95-4C6D-96A7-14002220E881}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="591" uniqueCount="381">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="621" uniqueCount="400">
   <si>
     <t>Timestamp</t>
   </si>
@@ -1238,6 +1238,63 @@
   </si>
   <si>
     <t>Did a example considering up time, output count and harmful alarms</t>
+  </si>
+  <si>
+    <t>Feb 27 10:00 to 11:00</t>
+  </si>
+  <si>
+    <t>Working with example of creating sample django site for PAM data exploration.</t>
+  </si>
+  <si>
+    <t>Feb 27 11:00 to 12:00</t>
+  </si>
+  <si>
+    <t>Created feature engineering class and used it to create features</t>
+  </si>
+  <si>
+    <t>Feb 27 12:00 to 13:00</t>
+  </si>
+  <si>
+    <t>Done modelling on data, used multi output regressor.</t>
+  </si>
+  <si>
+    <t>Feb 27 13:00 to 13:30</t>
+  </si>
+  <si>
+    <t>Working on tuning model</t>
+  </si>
+  <si>
+    <t>Feb 27 13:30 to 14:00</t>
+  </si>
+  <si>
+    <t>Feb 27 14:00 to 15:00</t>
+  </si>
+  <si>
+    <t>Ml phase done</t>
+  </si>
+  <si>
+    <t>Feb 27 15:00 to 16:00</t>
+  </si>
+  <si>
+    <t>Working on django backend</t>
+  </si>
+  <si>
+    <t>Feb 27 16:00 to 17:00</t>
+  </si>
+  <si>
+    <t>Done with sample example, using post making predictions.</t>
+  </si>
+  <si>
+    <t>Feb 27 17:00 to 18:00</t>
+  </si>
+  <si>
+    <t>Working on deploying classification problem.</t>
+  </si>
+  <si>
+    <t>Feb 27 18:00 to 19:00</t>
+  </si>
+  <si>
+    <t>Done demo ml example, deployed in django successfully</t>
   </si>
 </sst>
 </file>
@@ -1643,10 +1700,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07624C4B-536F-4CB7-AB8E-70C51D83A0BA}">
-  <dimension ref="A1:C218"/>
+  <dimension ref="A1:C229"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A195" workbookViewId="0">
-      <selection activeCell="D218" sqref="D218"/>
+    <sheetView tabSelected="1" topLeftCell="A210" workbookViewId="0">
+      <selection activeCell="B224" sqref="B224"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3928,6 +3985,121 @@
         <v>8</v>
       </c>
     </row>
+    <row r="219" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A219" s="5"/>
+      <c r="B219" s="6"/>
+      <c r="C219" s="5"/>
+    </row>
+    <row r="220" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A220" s="1" t="s">
+        <v>381</v>
+      </c>
+      <c r="B220" s="3" t="s">
+        <v>382</v>
+      </c>
+      <c r="C220" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="221" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A221" s="1" t="s">
+        <v>383</v>
+      </c>
+      <c r="B221" s="3" t="s">
+        <v>384</v>
+      </c>
+      <c r="C221" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="222" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A222" s="1" t="s">
+        <v>385</v>
+      </c>
+      <c r="B222" s="3" t="s">
+        <v>386</v>
+      </c>
+      <c r="C222" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="223" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A223" s="1" t="s">
+        <v>387</v>
+      </c>
+      <c r="B223" s="3" t="s">
+        <v>388</v>
+      </c>
+      <c r="C223" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="224" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A224" s="1" t="s">
+        <v>389</v>
+      </c>
+      <c r="B224" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C224" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="225" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A225" s="1" t="s">
+        <v>390</v>
+      </c>
+      <c r="B225" s="3" t="s">
+        <v>391</v>
+      </c>
+      <c r="C225" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="226" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A226" s="1" t="s">
+        <v>392</v>
+      </c>
+      <c r="B226" s="3" t="s">
+        <v>393</v>
+      </c>
+      <c r="C226" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="227" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A227" s="1" t="s">
+        <v>394</v>
+      </c>
+      <c r="B227" s="3" t="s">
+        <v>395</v>
+      </c>
+      <c r="C227" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="228" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A228" s="1" t="s">
+        <v>396</v>
+      </c>
+      <c r="B228" s="3" t="s">
+        <v>397</v>
+      </c>
+      <c r="C228" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="229" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A229" s="1" t="s">
+        <v>398</v>
+      </c>
+      <c r="B229" s="3" t="s">
+        <v>399</v>
+      </c>
+      <c r="C229" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Added timesheet and discussion of date 28-02-2020
</commit_message>
<xml_diff>
--- a/Timesheet January 2020.xlsx
+++ b/Timesheet January 2020.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\Timesheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44121EF9-DB72-4F1E-A8A5-548DFB04472C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D7B542B-D634-41A2-88A7-6BC24995CCC3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{4E06B61D-CC95-4C6D-96A7-14002220E881}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="621" uniqueCount="400">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="636" uniqueCount="408">
   <si>
     <t>Timestamp</t>
   </si>
@@ -1295,6 +1295,30 @@
   </si>
   <si>
     <t>Done demo ml example, deployed in django successfully</t>
+  </si>
+  <si>
+    <t>Feb 28 10:00 to 11:00</t>
+  </si>
+  <si>
+    <t>Stated model tuning, creating model tuning class, writing model tuning parameters.</t>
+  </si>
+  <si>
+    <t>Feb 28 11:00 to 12:30</t>
+  </si>
+  <si>
+    <t>Feb 28 12:30 to 13:30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Office anouncement and some documentations. </t>
+  </si>
+  <si>
+    <t>Feb 28 13:30 to 14:30</t>
+  </si>
+  <si>
+    <t>Feb 28 14:30 to 19:00</t>
+  </si>
+  <si>
+    <t>Python class and office work.</t>
   </si>
 </sst>
 </file>
@@ -1700,10 +1724,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07624C4B-536F-4CB7-AB8E-70C51D83A0BA}">
-  <dimension ref="A1:C229"/>
+  <dimension ref="A1:C235"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A210" workbookViewId="0">
-      <selection activeCell="B224" sqref="B224"/>
+    <sheetView tabSelected="1" topLeftCell="A214" workbookViewId="0">
+      <selection activeCell="D235" sqref="D235"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4100,6 +4124,66 @@
         <v>8</v>
       </c>
     </row>
+    <row r="230" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A230" s="5"/>
+      <c r="B230" s="6"/>
+      <c r="C230" s="5"/>
+    </row>
+    <row r="231" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A231" s="1" t="s">
+        <v>400</v>
+      </c>
+      <c r="B231" s="3" t="s">
+        <v>401</v>
+      </c>
+      <c r="C231" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="232" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A232" s="1" t="s">
+        <v>402</v>
+      </c>
+      <c r="B232" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C232" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="233" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A233" s="1" t="s">
+        <v>403</v>
+      </c>
+      <c r="B233" s="3" t="s">
+        <v>404</v>
+      </c>
+      <c r="C233" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="234" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A234" s="1" t="s">
+        <v>405</v>
+      </c>
+      <c r="B234" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C234" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="235" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A235" s="1" t="s">
+        <v>406</v>
+      </c>
+      <c r="B235" s="3" t="s">
+        <v>407</v>
+      </c>
+      <c r="C235" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Added timesheet of date 02-03-2020
</commit_message>
<xml_diff>
--- a/Timesheet January 2020.xlsx
+++ b/Timesheet January 2020.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\Timesheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D7B542B-D634-41A2-88A7-6BC24995CCC3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{994E39E4-71C5-4690-B153-ED2A2B18EE63}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{4E06B61D-CC95-4C6D-96A7-14002220E881}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="636" uniqueCount="408">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="663" uniqueCount="425">
   <si>
     <t>Timestamp</t>
   </si>
@@ -1319,6 +1319,58 @@
   </si>
   <si>
     <t>Python class and office work.</t>
+  </si>
+  <si>
+    <t>Mar 2 10:00 to 11:00</t>
+  </si>
+  <si>
+    <t>Build django backend for predicting automation time, failed units and output units</t>
+  </si>
+  <si>
+    <t>Mar 2 11:00 to 12:00</t>
+  </si>
+  <si>
+    <t>Working on transforming outfile dates</t>
+  </si>
+  <si>
+    <t>Mar 2 12:00 to 13:00</t>
+  </si>
+  <si>
+    <t>Discussion of project with frontend developer</t>
+  </si>
+  <si>
+    <t>Mar 2 13:00 to 14:00</t>
+  </si>
+  <si>
+    <t>Mar 2 14:00 to 15:00</t>
+  </si>
+  <si>
+    <t>Issues in transform output unit data, fixing issues</t>
+  </si>
+  <si>
+    <t>Mar 2 15:00 to 16:00</t>
+  </si>
+  <si>
+    <t>Resolving issue</t>
+  </si>
+  <si>
+    <t>Mar 2 16:00 to 17:00</t>
+  </si>
+  <si>
+    <t>Resolved issue, working on model building using new modifications</t>
+  </si>
+  <si>
+    <t>Mar 2 17:00 to 18:00</t>
+  </si>
+  <si>
+    <t>Model building done by modifying some code</t>
+  </si>
+  <si>
+    <t>Deployed model successfully, also implemented start time and end time logic
+successfully.</t>
+  </si>
+  <si>
+    <t>Mar 2 18:00 to 19:00</t>
   </si>
 </sst>
 </file>
@@ -1724,10 +1776,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07624C4B-536F-4CB7-AB8E-70C51D83A0BA}">
-  <dimension ref="A1:C235"/>
+  <dimension ref="A1:C245"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A214" workbookViewId="0">
-      <selection activeCell="D235" sqref="D235"/>
+    <sheetView tabSelected="1" topLeftCell="A218" workbookViewId="0">
+      <selection activeCell="B245" sqref="B245"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4184,6 +4236,110 @@
         <v>8</v>
       </c>
     </row>
+    <row r="236" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A236" s="5"/>
+      <c r="B236" s="6"/>
+      <c r="C236" s="5"/>
+    </row>
+    <row r="237" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A237" s="1" t="s">
+        <v>408</v>
+      </c>
+      <c r="B237" s="3" t="s">
+        <v>409</v>
+      </c>
+      <c r="C237" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="238" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A238" s="1" t="s">
+        <v>410</v>
+      </c>
+      <c r="B238" s="3" t="s">
+        <v>411</v>
+      </c>
+      <c r="C238" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="239" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A239" s="1" t="s">
+        <v>412</v>
+      </c>
+      <c r="B239" s="3" t="s">
+        <v>413</v>
+      </c>
+      <c r="C239" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="240" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A240" s="1" t="s">
+        <v>414</v>
+      </c>
+      <c r="B240" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C240" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="241" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A241" s="1" t="s">
+        <v>415</v>
+      </c>
+      <c r="B241" s="3" t="s">
+        <v>416</v>
+      </c>
+      <c r="C241" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="242" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A242" s="1" t="s">
+        <v>417</v>
+      </c>
+      <c r="B242" s="3" t="s">
+        <v>418</v>
+      </c>
+      <c r="C242" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="243" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A243" s="1" t="s">
+        <v>419</v>
+      </c>
+      <c r="B243" s="3" t="s">
+        <v>420</v>
+      </c>
+      <c r="C243" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="244" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A244" s="1" t="s">
+        <v>421</v>
+      </c>
+      <c r="B244" s="3" t="s">
+        <v>422</v>
+      </c>
+      <c r="C244" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="245" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A245" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="B245" s="2" t="s">
+        <v>423</v>
+      </c>
+      <c r="C245" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>